<commit_message>
creacion de la funcion de consultar tarea
</commit_message>
<xml_diff>
--- a/BaseCrudColab.xlsx
+++ b/BaseCrudColab.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -52,6 +52,36 @@
   </si>
   <si>
     <t>cantidad</t>
+  </si>
+  <si>
+    <t>gghg</t>
+  </si>
+  <si>
+    <t>tfyty</t>
+  </si>
+  <si>
+    <t>ftytg</t>
+  </si>
+  <si>
+    <t>tgyty</t>
+  </si>
+  <si>
+    <t>pendi</t>
+  </si>
+  <si>
+    <t>tff</t>
+  </si>
+  <si>
+    <t>gfgdf</t>
+  </si>
+  <si>
+    <t>eje</t>
+  </si>
+  <si>
+    <t>gfgd</t>
+  </si>
+  <si>
+    <t>dfg</t>
   </si>
 </sst>
 </file>
@@ -369,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +425,46 @@
       </c>
       <c r="F1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la funcion actualizar
</commit_message>
<xml_diff>
--- a/BaseCrudColab.xlsx
+++ b/BaseCrudColab.xlsx
@@ -1,75 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SENA\Tareas Danillo\BaseCrud_Trabajo colaborativo\gitflow_practica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja.tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="hoja.productos" sheetId="2" r:id="rId2"/>
+    <sheet name="hoja.tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="hoja.productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripción</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -88,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -368,66 +386,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descripción</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>daniel</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>frfr</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>finalizado</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>tgt</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>gt</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ejecucion</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>tgt</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>bbgb</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la funcion agregar
</commit_message>
<xml_diff>
--- a/BaseCrudColab.xlsx
+++ b/BaseCrudColab.xlsx
@@ -1,75 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SENA\Tareas Danillo\BaseCrud_Trabajo colaborativo\gitflow_practica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja.tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="hoja.productos" sheetId="2" r:id="rId2"/>
+    <sheet name="hoja.tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="hoja.productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripción</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -88,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -368,66 +386,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descripción</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>daniel</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>terminada</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la eliminacionde tareas
</commit_message>
<xml_diff>
--- a/BaseCrudColab.xlsx
+++ b/BaseCrudColab.xlsx
@@ -1,75 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SENA\Tareas Danillo\BaseCrud_Trabajo colaborativo\gitflow_practica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja.tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="hoja.productos" sheetId="2" r:id="rId2"/>
+    <sheet name="hoja.tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="hoja.productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripción</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -88,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -368,66 +386,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descripción</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
       </c>
     </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fin de los pull hacia daniel
</commit_message>
<xml_diff>
--- a/BaseCrudColab.xlsx
+++ b/BaseCrudColab.xlsx
@@ -1,105 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\SENA\Tareas Danillo\BaseCrud_Trabajo colaborativo\gitflow_practica\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja.tareas" sheetId="1" r:id="rId1"/>
-    <sheet name="hoja.productos" sheetId="2" r:id="rId2"/>
+    <sheet name="hoja.tareas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="hoja.productos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>descripción</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>categoria</t>
-  </si>
-  <si>
-    <t>precio</t>
-  </si>
-  <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>gghg</t>
-  </si>
-  <si>
-    <t>tfyty</t>
-  </si>
-  <si>
-    <t>ftytg</t>
-  </si>
-  <si>
-    <t>tgyty</t>
-  </si>
-  <si>
-    <t>pendi</t>
-  </si>
-  <si>
-    <t>tff</t>
-  </si>
-  <si>
-    <t>gfgdf</t>
-  </si>
-  <si>
-    <t>eje</t>
-  </si>
-  <si>
-    <t>gfgd</t>
-  </si>
-  <si>
-    <t>dfg</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -118,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -398,106 +386,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>descripción</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>fecha_inicio</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>fecha_fin</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>gghg</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>tfyty</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pendi</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ftytg</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>tgyty</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>tff</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>gfgdf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>eje</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>gfgd</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>sociales</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>En espera</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>18/2/2023</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>nombre</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>categoria</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>precio</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>cantidad</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creacion de la funcion de consultar producto
</commit_message>
<xml_diff>
--- a/BaseCrudColab.xlsx
+++ b/BaseCrudColab.xlsx
@@ -1,34 +1,118 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\gitflow_practica\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="hoja.tareas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="hoja.productos" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="hoja.tareas" sheetId="1" r:id="rId1"/>
+    <sheet name="hoja.productos" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>descripción</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+  </si>
+  <si>
+    <t>gghg</t>
+  </si>
+  <si>
+    <t>tfyty</t>
+  </si>
+  <si>
+    <t>pendi</t>
+  </si>
+  <si>
+    <t>ftytg</t>
+  </si>
+  <si>
+    <t>tgyty</t>
+  </si>
+  <si>
+    <t>tff</t>
+  </si>
+  <si>
+    <t>gfgdf</t>
+  </si>
+  <si>
+    <t>eje</t>
+  </si>
+  <si>
+    <t>gfgd</t>
+  </si>
+  <si>
+    <t>dfg</t>
+  </si>
+  <si>
+    <t>sociales</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>En espera</t>
+  </si>
+  <si>
+    <t>18/2/2023</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>precio</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>daniel</t>
+  </si>
+  <si>
+    <t>gei</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +131,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -386,136 +411,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nombre</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>descripción</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>estado</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>fecha_inicio</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>fecha_fin</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>gghg</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>tfyty</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>pendi</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>ftytg</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>tgyty</t>
-        </is>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>tff</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>gfgdf</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>eje</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>gfgd</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>dfg</t>
-        </is>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>sociales</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>En espera</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>18/2/2023</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -524,44 +504,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>nombre</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>categoria</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>precio</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>cantidad</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>